<commit_message>
Add support for xleta.unicode errors
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/UNICODE.xlsx
+++ b/xlsx/tests/calc_tests/UNICODE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\bruno\repos\IronCalc\xlsx\tests\calc_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08DBBE4-B12B-4A58-9357-190016C812F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB9E098-6928-47E5-BFDD-327A0DCEFE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{BE6270EA-F85F-4848-9581-55FBBFCF4D5D}"/>
   </bookViews>
@@ -37,6 +37,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -234,6 +256,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>7</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -723,7 +803,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC53CDA4-C07E-EE4C-AD72-581007D9709D}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
@@ -913,43 +993,52 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="e">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6" t="e" vm="1">
+        <f>_xleta.UNICODE</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="e">
         <f>B18</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B19" s="6" t="e">
-        <f t="shared" ref="B19:B21" si="1">_xlfn.UNICODE(A19)</f>
+      <c r="B20" s="6" t="e">
+        <f t="shared" ref="B20:B22" si="1">_xlfn.UNICODE(A20)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="str">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="str">
         <f>""</f>
         <v/>
       </c>
-      <c r="B20" s="6" t="e">
+      <c r="B21" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="e">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B21" s="6" t="e">
+      <c r="B22" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>